<commit_message>
Change paths of the parameter files, add the results of mask registration.
</commit_message>
<xml_diff>
--- a/output/exp_02.xlsx
+++ b/output/exp_02.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Fragkiadakis\Workspace\liver-baseline-registration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Fragkiadakis\Workspace\liver-baseline-registration\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7470BF9E-0F90-48F0-8337-3A4865156427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C38C6B-58B4-4FAA-ACAD-01B97EE71E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="480" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="3570" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,14 +98,29 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -135,11 +150,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,18 +461,18 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -484,22 +500,22 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.36810999999999999</v>
+        <v>0.38240000000000002</v>
       </c>
       <c r="C2">
-        <v>0.15187999999999999</v>
+        <v>0.20757999999999999</v>
       </c>
       <c r="D2">
-        <v>0.81728999999999996</v>
+        <v>0.81938999999999995</v>
       </c>
       <c r="E2">
-        <v>0.70777000000000001</v>
+        <v>0.64339999999999997</v>
       </c>
       <c r="F2">
-        <v>0.84408000000000005</v>
+        <v>0.84104000000000001</v>
       </c>
       <c r="G2">
-        <v>0.73658999999999997</v>
+        <v>0.69471000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -507,22 +523,22 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>4.5949999999999998E-2</v>
+        <v>4.9489999999999999E-2</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.8236</v>
+        <v>0.85614000000000001</v>
       </c>
       <c r="E3">
-        <v>0.86224999999999996</v>
+        <v>0.84455999999999998</v>
       </c>
       <c r="F3">
-        <v>0.82926</v>
+        <v>0.85511999999999999</v>
       </c>
       <c r="G3">
-        <v>0.86499000000000004</v>
+        <v>0.84243000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -530,22 +546,22 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.25006</v>
+        <v>0.30375999999999997</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.81428999999999996</v>
+        <v>0.88461000000000001</v>
       </c>
       <c r="E4">
-        <v>0.61260000000000003</v>
+        <v>0.76642999999999994</v>
       </c>
       <c r="F4">
-        <v>0.83367999999999998</v>
+        <v>0.88099000000000005</v>
       </c>
       <c r="G4">
-        <v>0.63017000000000001</v>
+        <v>0.72480999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -553,22 +569,22 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.37913999999999998</v>
+        <v>0.40884999999999999</v>
       </c>
       <c r="C5">
-        <v>0.30259999999999998</v>
+        <v>0.27077000000000001</v>
       </c>
       <c r="D5">
-        <v>0.92152000000000001</v>
+        <v>0.93189</v>
       </c>
       <c r="E5">
-        <v>0.91142999999999996</v>
+        <v>0.94987999999999995</v>
       </c>
       <c r="F5">
-        <v>0.93100000000000005</v>
+        <v>0.93078000000000005</v>
       </c>
       <c r="G5">
-        <v>0.91922999999999999</v>
+        <v>0.94355</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -582,16 +598,16 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.84899000000000002</v>
+        <v>0.87812000000000001</v>
       </c>
       <c r="E6">
-        <v>0.72448000000000001</v>
+        <v>0.87246000000000001</v>
       </c>
       <c r="F6">
-        <v>0.86170000000000002</v>
+        <v>0.872</v>
       </c>
       <c r="G6">
-        <v>0.74087000000000003</v>
+        <v>0.86456</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -599,22 +615,22 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>2.562E-2</v>
+        <v>3.653E-2</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.82840999999999998</v>
+        <v>0.56352000000000002</v>
       </c>
       <c r="E7">
-        <v>0.21168999999999999</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0.84397</v>
+        <v>0.56145999999999996</v>
       </c>
       <c r="G7">
-        <v>0.22961999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -622,22 +638,22 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.47952</v>
+        <v>0.38774999999999998</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0.79627999999999999</v>
+        <v>0.74173999999999995</v>
       </c>
       <c r="E8">
-        <v>0.52390000000000003</v>
+        <v>0.70555000000000001</v>
       </c>
       <c r="F8">
-        <v>0.80093999999999999</v>
+        <v>0.73912999999999995</v>
       </c>
       <c r="G8">
-        <v>0.52393999999999996</v>
+        <v>0.68742000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -645,22 +661,22 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>0.20066000000000001</v>
+        <v>0.24389</v>
       </c>
       <c r="C9">
-        <v>0.13896</v>
+        <v>0.14654</v>
       </c>
       <c r="D9">
-        <v>0.82559000000000005</v>
+        <v>0.66715999999999998</v>
       </c>
       <c r="E9">
-        <v>0.69886000000000004</v>
+        <v>0.64102000000000003</v>
       </c>
       <c r="F9">
-        <v>0.83733999999999997</v>
+        <v>0.66966000000000003</v>
       </c>
       <c r="G9">
-        <v>0.71721000000000001</v>
+        <v>0.64731000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -668,22 +684,22 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>0.50329999999999997</v>
+        <v>0.46000999999999997</v>
       </c>
       <c r="C10">
-        <v>0.26251999999999998</v>
+        <v>0.31574000000000002</v>
       </c>
       <c r="D10">
-        <v>0.88644000000000001</v>
+        <v>0.82872999999999997</v>
       </c>
       <c r="E10">
-        <v>0.85841000000000001</v>
+        <v>0.77553000000000005</v>
       </c>
       <c r="F10">
-        <v>0.88846000000000003</v>
+        <v>0.83130999999999999</v>
       </c>
       <c r="G10">
-        <v>0.86116000000000004</v>
+        <v>0.77678999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -691,22 +707,22 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>0.15003</v>
+        <v>0.14257</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0.79571999999999998</v>
+        <v>0.78188999999999997</v>
       </c>
       <c r="E11">
-        <v>0.58140000000000003</v>
+        <v>0.61377000000000004</v>
       </c>
       <c r="F11">
-        <v>0.80154000000000003</v>
+        <v>0.79803000000000002</v>
       </c>
       <c r="G11">
-        <v>0.58577999999999997</v>
+        <v>0.62234</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -720,16 +736,16 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.79571999999999998</v>
+        <v>0.56352000000000002</v>
       </c>
       <c r="E12">
-        <v>0.21168999999999999</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0.80093999999999999</v>
+        <v>0.56145999999999996</v>
       </c>
       <c r="G12">
-        <v>0.22961999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -737,22 +753,22 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>0.50329999999999997</v>
+        <v>0.46000999999999997</v>
       </c>
       <c r="C13">
-        <v>0.30259999999999998</v>
+        <v>0.31574000000000002</v>
       </c>
       <c r="D13">
-        <v>0.92152000000000001</v>
+        <v>0.93189</v>
       </c>
       <c r="E13">
-        <v>0.91142999999999996</v>
+        <v>0.94987999999999995</v>
       </c>
       <c r="F13">
-        <v>0.93100000000000005</v>
+        <v>0.93078000000000005</v>
       </c>
       <c r="G13">
-        <v>0.91922999999999999</v>
+        <v>0.94355</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -760,22 +776,22 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>0.24214083333333331</v>
+        <v>0.23960500000000001</v>
       </c>
       <c r="C14">
-        <v>9.654666666666667E-2</v>
+        <v>0.1046975</v>
       </c>
       <c r="D14">
-        <v>0.83961416666666644</v>
+        <v>0.78738333333333321</v>
       </c>
       <c r="E14">
-        <v>0.65132583333333338</v>
-      </c>
-      <c r="F14">
-        <v>0.85032583333333334</v>
+        <v>0.6468733333333333</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.78931333333333331</v>
       </c>
       <c r="G14">
-        <v>0.66320083333333324</v>
+        <v>0.6456225000000001</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -783,22 +799,22 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>0.24214083333333331</v>
+        <v>0.24389</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0.82559000000000005</v>
+        <v>0.81938999999999995</v>
       </c>
       <c r="E15">
-        <v>0.69886000000000004</v>
+        <v>0.70555000000000001</v>
       </c>
       <c r="F15">
-        <v>0.84397</v>
+        <v>0.83130999999999999</v>
       </c>
       <c r="G15">
-        <v>0.71721000000000001</v>
+        <v>0.69471000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>